<commit_message>
fitness and precision update
</commit_message>
<xml_diff>
--- a/BPI 2013/fitness.xlsx
+++ b/BPI 2013/fitness.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\process mining\pm4py\BPI 2013\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7B352B-44FE-4865-870F-987D87D9BD3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A690B0D-1F3E-4E02-BAAE-75F80B502499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07B94767-5DC1-4B3B-9FBC-0F9B4C71E218}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>cluster 2</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>running time(seconds)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>precision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>log-based precision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fitness</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -445,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72D3A8B-AC97-456B-8DE4-BA101B779A00}">
-  <dimension ref="B6:I24"/>
+  <dimension ref="B6:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="O16" sqref="O15:O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -457,7 +469,7 @@
     <col min="6" max="7" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>1</v>
       </c>
@@ -467,8 +479,17 @@
       <c r="I6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -487,8 +508,18 @@
       <c r="I7">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>0.43469999999999998</v>
+      </c>
+      <c r="O7">
+        <f>M7*2</f>
+        <v>0.86939999999999995</v>
+      </c>
+      <c r="R7">
+        <v>0.94359999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>5</v>
       </c>
@@ -501,8 +532,18 @@
       <c r="I8">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>0.4</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8:O24" si="0">M8*2</f>
+        <v>0.8</v>
+      </c>
+      <c r="R8">
+        <v>0.95420000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>6</v>
       </c>
@@ -518,8 +559,18 @@
       <c r="I9">
         <v>99</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>0.43469999999999998</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>0.86939999999999995</v>
+      </c>
+      <c r="R9">
+        <v>0.94479999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>5</v>
       </c>
@@ -532,8 +583,18 @@
       <c r="I10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>0.25</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="R10">
+        <v>0.99209999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>8</v>
       </c>
@@ -546,8 +607,18 @@
       <c r="I11">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>0.4</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="R11">
+        <v>0.92779999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>9</v>
       </c>
@@ -563,8 +634,18 @@
       <c r="I12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>0.3</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="R12">
+        <v>0.94630000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>4</v>
       </c>
@@ -577,8 +658,18 @@
       <c r="I13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>0.4</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>7</v>
       </c>
@@ -591,8 +682,18 @@
       <c r="I14">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="R14">
+        <v>0.92720000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>10</v>
       </c>
@@ -605,8 +706,18 @@
       <c r="I15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>0.3</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="R15">
+        <v>0.99819999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -625,8 +736,18 @@
       <c r="I16">
         <v>116</v>
       </c>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>0.47820000000000001</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>0.95640000000000003</v>
+      </c>
+      <c r="R16">
+        <v>0.95299999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>5</v>
       </c>
@@ -639,8 +760,18 @@
       <c r="I17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>6</v>
       </c>
@@ -656,8 +787,18 @@
       <c r="I18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>5</v>
       </c>
@@ -670,8 +811,18 @@
       <c r="I19">
         <v>125</v>
       </c>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>0.47820000000000001</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="0"/>
+        <v>0.95640000000000003</v>
+      </c>
+      <c r="R19">
+        <v>0.95650000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>8</v>
       </c>
@@ -684,8 +835,18 @@
       <c r="I20">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>9</v>
       </c>
@@ -701,8 +862,18 @@
       <c r="I21">
         <v>126</v>
       </c>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>0.47820000000000001</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="0"/>
+        <v>0.95640000000000003</v>
+      </c>
+      <c r="R21">
+        <v>0.94750000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>4</v>
       </c>
@@ -715,8 +886,18 @@
       <c r="I22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>7</v>
       </c>
@@ -729,8 +910,18 @@
       <c r="I23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>10</v>
       </c>
@@ -741,6 +932,16 @@
         <v>0.87559523809523798</v>
       </c>
       <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R24">
         <v>1</v>
       </c>
     </row>

</xml_diff>